<commit_message>
updated with angus understandability score
</commit_message>
<xml_diff>
--- a/documents/Design/Sufficiency&Understandability.xlsx
+++ b/documents/Design/Sufficiency&Understandability.xlsx
@@ -1624,7 +1624,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,7 +1689,7 @@
         <v>11</v>
       </c>
       <c r="G7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1756,7 +1756,7 @@
       </c>
       <c r="G12" s="1">
         <f>AVERAGE(G6:G10)</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated understandability with Brandon's sscore
</commit_message>
<xml_diff>
--- a/documents/Design/Sufficiency&Understandability.xlsx
+++ b/documents/Design/Sufficiency&Understandability.xlsx
@@ -1624,7 +1624,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,7 +1706,7 @@
         <v>12</v>
       </c>
       <c r="G8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1756,7 +1756,7 @@
       </c>
       <c r="G12" s="1">
         <f>AVERAGE(G6:G10)</f>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated understandability metric for new dashboard wireframe
</commit_message>
<xml_diff>
--- a/documents/Design/Sufficiency&Understandability.xlsx
+++ b/documents/Design/Sufficiency&Understandability.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="StateTransition" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="15">
   <si>
     <t>Sufficiency</t>
   </si>
@@ -132,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -141,6 +141,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1174,15 +1175,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="2" max="2" width="50.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" customWidth="1"/>
@@ -1323,9 +1324,135 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D14" s="4">
+        <v>42693</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.33</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1">
+        <f>AVERAGE(B18:B22)</f>
+        <v>0.35933333333333334</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="1">
+        <f>AVERAGE(G18:G22)</f>
+        <v>0.4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1623,7 +1750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated with angus understandability
</commit_message>
<xml_diff>
--- a/documents/Design/Sufficiency&Understandability.xlsx
+++ b/documents/Design/Sufficiency&Understandability.xlsx
@@ -1177,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,7 +1380,7 @@
         <v>11</v>
       </c>
       <c r="G19" s="5">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="G24" s="1">
         <f>AVERAGE(G18:G22)</f>
-        <v>0.4</v>
+        <v>0.55999999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated understandability metric w/ brandon & yash
</commit_message>
<xml_diff>
--- a/documents/Design/Sufficiency&Understandability.xlsx
+++ b/documents/Design/Sufficiency&Understandability.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="StateTransition" sheetId="1" r:id="rId1"/>
@@ -1177,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,7 +1397,7 @@
         <v>12</v>
       </c>
       <c r="G20" s="5">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1431,7 +1431,7 @@
         <v>14</v>
       </c>
       <c r="G22" s="5">
-        <v>0</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1447,7 +1447,7 @@
       </c>
       <c r="G24" s="1">
         <f>AVERAGE(G18:G22)</f>
-        <v>0.55999999999999994</v>
+        <v>0.89</v>
       </c>
     </row>
   </sheetData>
@@ -1750,7 +1750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -1867,7 +1867,7 @@
         <v>14</v>
       </c>
       <c r="G10" s="5">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="G12" s="1">
         <f>AVERAGE(G6:G10)</f>
-        <v>0.8</v>
+        <v>0.98000000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated understandability design metric.
</commit_message>
<xml_diff>
--- a/documents/Design/Sufficiency&Understandability.xlsx
+++ b/documents/Design/Sufficiency&Understandability.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="StateTransition" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="15">
   <si>
     <t>Sufficiency</t>
   </si>
@@ -1603,10 +1603,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,6 +1741,130 @@
         <v>0.6</v>
       </c>
     </row>
+    <row r="15" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D15" s="4">
+        <v>42709</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="5">
+        <v>0</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="1">
+        <f>AVERAGE(B20:B24)</f>
+        <v>0.2533333333333333</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="1">
+        <f>AVERAGE(G20:G24)</f>
+        <v>0.80999999999999994</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1750,7 +1874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
created single document for metrics charts & graphs
</commit_message>
<xml_diff>
--- a/documents/Design/Sufficiency&Understandability.xlsx
+++ b/documents/Design/Sufficiency&Understandability.xlsx
@@ -110,7 +110,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -173,7 +173,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -268,87 +268,81 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Charts!$B$2</c:f>
+              <c:f>Charts!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>State Transition</c:v>
+                  <c:v>2-Nov</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Charts!$A$3:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
+            <c:strRef>
+              <c:f>Charts!$B$2:$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>42676</c:v>
+                  <c:v>State Transition</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42682</c:v>
+                  <c:v>Use Case</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42691</c:v>
+                  <c:v>System Design</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42693</c:v>
+                  <c:v>Dash Board</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Login</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>New Post</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sign Up</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$B$3:$B$7</c:f>
+              <c:f>Charts!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8</c:v>
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F447-4FCE-9DD4-F0205A73FE8D}"/>
@@ -360,79 +354,81 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Charts!$C$2</c:f>
+              <c:f>Charts!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Use Case</c:v>
+                  <c:v>8-Nov</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Charts!$A$3:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
+            <c:strRef>
+              <c:f>Charts!$B$2:$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>42676</c:v>
+                  <c:v>State Transition</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42682</c:v>
+                  <c:v>Use Case</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42691</c:v>
+                  <c:v>System Design</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42693</c:v>
+                  <c:v>Dash Board</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Login</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>New Post</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sign Up</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$C$3:$C$7</c:f>
+              <c:f>Charts!$B$4:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.73</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F447-4FCE-9DD4-F0205A73FE8D}"/>
@@ -444,79 +440,66 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Charts!$D$2</c:f>
+              <c:f>Charts!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>System Design</c:v>
+                  <c:v>17-Nov</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Charts!$A$3:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
+            <c:strRef>
+              <c:f>Charts!$B$2:$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>42676</c:v>
+                  <c:v>State Transition</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42682</c:v>
+                  <c:v>Use Case</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42691</c:v>
+                  <c:v>System Design</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42693</c:v>
+                  <c:v>Dash Board</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Login</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>New Post</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sign Up</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$D$3:$D$7</c:f>
+              <c:f>Charts!$B$5:$H$5</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.79</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="6" formatCode="0%">
+                  <c:v>0.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-F447-4FCE-9DD4-F0205A73FE8D}"/>
@@ -528,79 +511,66 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Charts!$E$2</c:f>
+              <c:f>Charts!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Dash Board</c:v>
+                  <c:v>19-Nov</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Charts!$A$3:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
+            <c:strRef>
+              <c:f>Charts!$B$2:$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>42676</c:v>
+                  <c:v>State Transition</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42682</c:v>
+                  <c:v>Use Case</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42691</c:v>
+                  <c:v>System Design</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42693</c:v>
+                  <c:v>Dash Board</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Login</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>New Post</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sign Up</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$E$3:$E$7</c:f>
+              <c:f>Charts!$B$6:$H$6</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="3" formatCode="0%">
                   <c:v>0.36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-F447-4FCE-9DD4-F0205A73FE8D}"/>
@@ -612,250 +582,69 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Charts!$F$2</c:f>
+              <c:f>Charts!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Login</c:v>
+                  <c:v>5-Dec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Charts!$A$3:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
+            <c:strRef>
+              <c:f>Charts!$B$2:$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>42676</c:v>
+                  <c:v>State Transition</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42682</c:v>
+                  <c:v>Use Case</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42691</c:v>
+                  <c:v>System Design</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42693</c:v>
+                  <c:v>Dash Board</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Login</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>New Post</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sign Up</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$F$3:$F$7</c:f>
+              <c:f>Charts!$B$7:$H$7</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>0.23</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="5" formatCode="0%">
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-F447-4FCE-9DD4-F0205A73FE8D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Charts!$G$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>New Post</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Charts!$A$3:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>42676</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42682</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42691</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42693</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Charts!$G$3:$G$7</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.25</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-F447-4FCE-9DD4-F0205A73FE8D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Charts!$H$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Sign Up</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Charts!$A$3:$A$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>42676</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42682</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42691</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42693</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Charts!$H$3:$H$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="2" formatCode="0%">
-                  <c:v>0.05</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-F447-4FCE-9DD4-F0205A73FE8D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -867,19 +656,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
+        <c:gapWidth val="150"/>
         <c:axId val="311566400"/>
         <c:axId val="311566728"/>
-      </c:lineChart>
-      <c:dateAx>
+      </c:barChart>
+      <c:catAx>
         <c:axId val="311566400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="[$-409]d\-mmm;@" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -919,9 +707,10 @@
         <c:crossAx val="311566728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="311566728"/>
         <c:scaling>
@@ -1186,87 +975,81 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Charts!$L$2</c:f>
+              <c:f>Charts!$K$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>State Transition</c:v>
+                  <c:v>2-Nov</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Charts!$K$3:$K$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
+            <c:strRef>
+              <c:f>Charts!$L$2:$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>42676</c:v>
+                  <c:v>State Transition</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42682</c:v>
+                  <c:v>Use Case</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42691</c:v>
+                  <c:v>System Design</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42693</c:v>
+                  <c:v>Dash Board</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Login</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>New Post</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sign Up</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$L$3:$L$7</c:f>
+              <c:f>Charts!$L$3:$R$3</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.88</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.84</c:v>
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0678-49CB-96E6-2D390521270C}"/>
@@ -1278,79 +1061,81 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Charts!$M$2</c:f>
+              <c:f>Charts!$K$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Use Case</c:v>
+                  <c:v>8-Nov</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Charts!$K$3:$K$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
+            <c:strRef>
+              <c:f>Charts!$L$2:$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>42676</c:v>
+                  <c:v>State Transition</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42682</c:v>
+                  <c:v>Use Case</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42691</c:v>
+                  <c:v>System Design</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42693</c:v>
+                  <c:v>Dash Board</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Login</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>New Post</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sign Up</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$M$3:$M$7</c:f>
+              <c:f>Charts!$L$4:$R$4</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.38</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-0678-49CB-96E6-2D390521270C}"/>
@@ -1362,79 +1147,66 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Charts!$N$2</c:f>
+              <c:f>Charts!$K$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>System Design</c:v>
+                  <c:v>17-Nov</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Charts!$K$3:$K$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
+            <c:strRef>
+              <c:f>Charts!$L$2:$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>42676</c:v>
+                  <c:v>State Transition</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42682</c:v>
+                  <c:v>Use Case</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42691</c:v>
+                  <c:v>System Design</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42693</c:v>
+                  <c:v>Dash Board</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Login</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>New Post</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sign Up</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$N$3:$N$7</c:f>
+              <c:f>Charts!$L$5:$R$5</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.38</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.86</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="6" formatCode="0%">
+                  <c:v>0.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-0678-49CB-96E6-2D390521270C}"/>
@@ -1446,79 +1218,66 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Charts!$O$2</c:f>
+              <c:f>Charts!$K$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Dash Board</c:v>
+                  <c:v>19-Nov</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Charts!$K$3:$K$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
+            <c:strRef>
+              <c:f>Charts!$L$2:$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>42676</c:v>
+                  <c:v>State Transition</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42682</c:v>
+                  <c:v>Use Case</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42691</c:v>
+                  <c:v>System Design</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42693</c:v>
+                  <c:v>Dash Board</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Login</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>New Post</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sign Up</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$O$3:$O$7</c:f>
+              <c:f>Charts!$L$6:$R$6</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>0.94</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="3" formatCode="0%">
                   <c:v>0.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-0678-49CB-96E6-2D390521270C}"/>
@@ -1530,250 +1289,69 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Charts!$P$2</c:f>
+              <c:f>Charts!$K$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Login</c:v>
+                  <c:v>5-Dec</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Charts!$K$3:$K$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
+            <c:strRef>
+              <c:f>Charts!$L$2:$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>42676</c:v>
+                  <c:v>State Transition</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42682</c:v>
+                  <c:v>Use Case</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42691</c:v>
+                  <c:v>System Design</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42693</c:v>
+                  <c:v>Dash Board</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Login</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>New Post</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Sign Up</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Charts!$P$3:$P$7</c:f>
+              <c:f>Charts!$L$7:$R$7</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>0.8</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="5" formatCode="0%">
+                  <c:v>0.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-0678-49CB-96E6-2D390521270C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Charts!$Q$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>New Post</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Charts!$K$3:$K$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>42676</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42682</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42691</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42693</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Charts!$Q$3:$Q$7</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.81</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-0678-49CB-96E6-2D390521270C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Charts!$R$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Sign Up</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Charts!$K$3:$K$7</c:f>
-              <c:numCache>
-                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>42676</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>42682</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42691</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>42693</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42709</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Charts!$R$3:$R$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="2" formatCode="0%">
-                  <c:v>0.98</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-0678-49CB-96E6-2D390521270C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1785,19 +1363,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
+        <c:gapWidth val="150"/>
         <c:axId val="388218264"/>
         <c:axId val="388215312"/>
-      </c:lineChart>
-      <c:dateAx>
+      </c:barChart>
+      <c:catAx>
         <c:axId val="388218264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="[$-409]d\-mmm;@" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1837,9 +1414,10 @@
         <c:crossAx val="388215312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="388215312"/>
         <c:scaling>
@@ -3502,8 +3080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>